<commit_message>
Add Excel file column headings
</commit_message>
<xml_diff>
--- a/People.xlsx
+++ b/People.xlsx
@@ -11,16 +11,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Parties</t>
+  </si>
+  <si>
+    <t>Example person</t>
+  </si>
+  <si>
+    <t>072 042 2222</t>
+  </si>
+  <si>
+    <t>test@example.com</t>
+  </si>
+  <si>
+    <t>EFF, DA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -30,6 +51,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -45,11 +67,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -272,6 +300,29 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>